<commit_message>
MVP of irt0  model class
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">A</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J</t>
   </si>
 </sst>
 </file>
@@ -61,6 +64,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -81,6 +85,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -155,13 +160,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
+      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -195,6 +200,9 @@
       <c r="K1" s="2" t="n">
         <v>10</v>
       </c>
+      <c r="L1" s="0" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -230,6 +238,9 @@
       <c r="K2" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="L2" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -264,6 +275,9 @@
       </c>
       <c r="K3" s="2" t="n">
         <v>0</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -300,6 +314,9 @@
       <c r="K4" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="L4" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
@@ -335,6 +352,9 @@
       <c r="K5" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="L5" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
@@ -370,6 +390,9 @@
       <c r="K6" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="L6" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -405,6 +428,9 @@
       <c r="K7" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="L7" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
@@ -440,6 +466,9 @@
       <c r="K8" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="L8" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
@@ -475,6 +504,9 @@
       <c r="K9" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="L9" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
@@ -509,6 +541,47 @@
       </c>
       <c r="K10" s="2" t="n">
         <v>0</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>